<commit_message>
cleaned up DRC schematic errors, assigned original footprints schematics
</commit_message>
<xml_diff>
--- a/badge2023-bom-r1.xlsx
+++ b/badge2023-bom-r1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66812F78-9F48-394E-A91D-C6162CB022E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF027756-99E4-8A43-BB99-52929AA4107C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -947,8 +947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>

</xml_diff>